<commit_message>
map & ring position
</commit_message>
<xml_diff>
--- a/решения/WORLD.xlsx
+++ b/решения/WORLD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reynikovanton/Desktop/APP/development/Locity/решения/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DFA169-DF60-4143-9C4F-A25E7DFB279D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B7E65C-929C-2542-BD79-055E0F95D69E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13000" yWindow="2200" windowWidth="32140" windowHeight="18400" xr2:uid="{7A1DAF9C-3E66-3A48-9BB9-B43E45C7788D}"/>
+    <workbookView xWindow="13000" yWindow="2200" windowWidth="32140" windowHeight="18400" activeTab="1" xr2:uid="{7A1DAF9C-3E66-3A48-9BB9-B43E45C7788D}"/>
   </bookViews>
   <sheets>
     <sheet name="Continents" sheetId="1" r:id="rId1"/>
@@ -840,9 +840,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE97BFD-F36A-4E40-AD7D-EA1A19204B91}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1177,9 +1177,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BADC1B24-763A-458E-B6D6-B0F23F0AB5F5}">
   <dimension ref="A1:AZ332"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>